<commit_message>
updated shops form for excel
</commit_message>
<xml_diff>
--- a/iiest_web/src/assets/foscos.csv.xlsx
+++ b/iiest_web/src/assets/foscos.csv.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2f3cda7c535a5681/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Angular\iiest\iiest\iiest_web\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B06665B7-4EAC-4518-8E3E-2ADDF4D33E6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04C39FBB-6491-43B6-A8F6-E3E207C26ACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{DB7A2692-9445-4062-9C2E-9BC095D4E044}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DB7A2692-9445-4062-9C2E-9BC095D4E044}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,12 +34,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>operatorName</t>
   </si>
   <si>
     <t>address</t>
+  </si>
+  <si>
+    <t>pincode</t>
+  </si>
+  <si>
+    <t>village</t>
+  </si>
+  <si>
+    <t>tehsil</t>
   </si>
 </sst>
 </file>
@@ -401,26 +410,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBF0DC7F-5E4E-4951-B73A-4B462181FA80}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1"/>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>